<commit_message>
Actualizar archivo base_de_datos.xlsx con contenido nuevo
</commit_message>
<xml_diff>
--- a/base_de_datos.xlsx
+++ b/base_de_datos.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="10.105.227.52551"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="590" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors/>
+  <commentList/>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -56,44 +64,367 @@
   </si>
   <si>
     <t>maria@yahoo.com</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Roque</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Leticia</t>
+  </si>
+  <si>
+    <t>Tejo</t>
+  </si>
+  <si>
+    <t>Jose Luis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
-    <font>
-      <sz val="11"/>
+  <numFmts count="0"/>
+  <fonts count="20">
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="10"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="11"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <sz val="18.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="3"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F76"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF3F3F3F"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FFFA7D00"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF006100"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C0006"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF9C6500"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color theme="0"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+      <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -108,23 +439,321 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399980"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyAlignment="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
+    <cellStyle name="20% - Acento1" xfId="25" builtinId="30"/>
+    <cellStyle name="20% - Acento2" xfId="29" builtinId="34"/>
+    <cellStyle name="20% - Acento3" xfId="33" builtinId="38"/>
+    <cellStyle name="20% - Acento4" xfId="37" builtinId="42"/>
+    <cellStyle name="20% - Acento5" xfId="41" builtinId="46"/>
+    <cellStyle name="20% - Acento6" xfId="45" builtinId="50"/>
+    <cellStyle name="40% - Acento1" xfId="26" builtinId="31"/>
+    <cellStyle name="40% - Acento2" xfId="30" builtinId="35"/>
+    <cellStyle name="40% - Acento3" xfId="34" builtinId="39"/>
+    <cellStyle name="40% - Acento4" xfId="38" builtinId="43"/>
+    <cellStyle name="40% - Acento5" xfId="42" builtinId="47"/>
+    <cellStyle name="40% - Acento6" xfId="46" builtinId="51"/>
+    <cellStyle name="60% - Acento1" xfId="27" builtinId="32"/>
+    <cellStyle name="60% - Acento2" xfId="31" builtinId="36"/>
+    <cellStyle name="60% - Acento3" xfId="35" builtinId="40"/>
+    <cellStyle name="60% - Acento4" xfId="39" builtinId="44"/>
+    <cellStyle name="60% - Acento5" xfId="43" builtinId="48"/>
+    <cellStyle name="60% - Acento6" xfId="47" builtinId="52"/>
+    <cellStyle name="Acento1" xfId="24" builtinId="29"/>
+    <cellStyle name="Acento2" xfId="28" builtinId="33"/>
+    <cellStyle name="Acento3" xfId="32" builtinId="37"/>
+    <cellStyle name="Acento4" xfId="36" builtinId="41"/>
+    <cellStyle name="Acento5" xfId="40" builtinId="45"/>
+    <cellStyle name="Acento6" xfId="44" builtinId="49"/>
+    <cellStyle name="Buena" xfId="21" builtinId="26"/>
+    <cellStyle name="Celda de comprobación" xfId="18" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="19" builtinId="24"/>
+    <cellStyle name="Coma" xfId="1" builtinId="3"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Comentario" xfId="8" builtinId="10"/>
+    <cellStyle name="Cálculo" xfId="17" builtinId="22"/>
+    <cellStyle name="Entrada" xfId="15" builtinId="20"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Incorrecto" xfId="22" builtinId="27"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Neutral" xfId="23" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
+    <cellStyle name="Salida" xfId="16" builtinId="21"/>
+    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
+    <cellStyle name="Texto explicativo" xfId="48" builtinId="53"/>
+    <cellStyle name="Total" xfId="20" builtinId="25"/>
+    <cellStyle name="Título" xfId="10" builtinId="15"/>
+    <cellStyle name="Título 1" xfId="11" builtinId="16"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Título 3" xfId="13" builtinId="18"/>
+    <cellStyle name="Título 4" xfId="14" builtinId="19"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -413,11 +1042,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.000000"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -437,57 +1068,128 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="0">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0">
+        <v>25</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0">
+        <v>25</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="0">
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>